<commit_message>
Class variable criteria in english and some minor adjustments.
</commit_message>
<xml_diff>
--- a/class_variable_criteria.xlsx
+++ b/class_variable_criteria.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alvaro C\Dropbox\1. Escritos\1. Artículos\1 2023_Estallido Social, malestar material y protesta\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alvaro C\Dropbox\3. Educacion\1. MA_LACIS\Lacis_MA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E5D5B04-0896-4274-B93A-3336445B4192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2889A436-D5D5-4016-977F-C6C8B188CC57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,22 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="24">
-  <si>
-    <t>Autoempleo</t>
-  </si>
-  <si>
-    <t>Num. Empleados</t>
-  </si>
-  <si>
-    <t>Supervisa</t>
-  </si>
-  <si>
-    <t>Resultados</t>
-  </si>
-  <si>
-    <t>Sí</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="20">
   <si>
     <t>10+</t>
   </si>
@@ -48,63 +33,74 @@
     <t>-</t>
   </si>
   <si>
-    <t>Burguesía tradicional</t>
-  </si>
-  <si>
-    <t>sí</t>
-  </si>
-  <si>
-    <t>2 a 10</t>
-  </si>
-  <si>
-    <t>Pequeño empleador</t>
-  </si>
-  <si>
-    <t>0 a 2</t>
-  </si>
-  <si>
-    <t>Pequeña burguesía</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
-    <t>Credencial</t>
-  </si>
-  <si>
-    <t>Directivo/Supervisor Experto (BA)</t>
-  </si>
-  <si>
-    <t>Proletario tradicional</t>
-  </si>
-  <si>
-    <t>Tipo empresa</t>
-  </si>
-  <si>
-    <t>Sí (BA+)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Experto (BA+) No directivo </t>
-  </si>
-  <si>
-    <t>Sí (-BA)</t>
-  </si>
-  <si>
-    <t>Directivo/Supervisor Semi-Credencializado</t>
-  </si>
-  <si>
-    <t>Obrero semi-credencializado</t>
-  </si>
-  <si>
-    <t>Directivo/Supervisor no credencializado</t>
+    <t>Self-employment</t>
+  </si>
+  <si>
+    <t>Number of employees</t>
+  </si>
+  <si>
+    <t>Skills</t>
+  </si>
+  <si>
+    <t>Supervises</t>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burgeoisie </t>
+  </si>
+  <si>
+    <t>Small Employers</t>
+  </si>
+  <si>
+    <t>Petty Burgeoisie</t>
+  </si>
+  <si>
+    <t>Expert Managers</t>
+  </si>
+  <si>
+    <t>Expert non-managers</t>
+  </si>
+  <si>
+    <t>Semi-credential managers</t>
+  </si>
+  <si>
+    <t>Semi-credential workers</t>
+  </si>
+  <si>
+    <t>Non-credential manager</t>
+  </si>
+  <si>
+    <t>Traditional proletarial</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>2 to 10</t>
+  </si>
+  <si>
+    <t>0 to 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -132,9 +128,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,192 +419,188 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.85546875" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" t="s">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>